<commit_message>
Some test code added to test_code.py
</commit_message>
<xml_diff>
--- a/data_table.xlsx
+++ b/data_table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/d3c3pt10n/Programming/Python/Vilkeen/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Harry\Programming\Vilkeen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6179DE8F-910F-0847-96CA-32F9FF359A50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D71898B-5194-4BDC-A7D6-92CE2370A553}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" tabRatio="615" xr2:uid="{E8BF67C5-1EE1-41FF-B76F-515721DCE47B}"/>
+    <workbookView xWindow="-19305" yWindow="0" windowWidth="19410" windowHeight="15585" tabRatio="673" xr2:uid="{E8BF67C5-1EE1-41FF-B76F-515721DCE47B}"/>
   </bookViews>
   <sheets>
     <sheet name="player" sheetId="11" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="51">
   <si>
     <t>id</t>
   </si>
@@ -212,7 +212,13 @@
     <t>buffs</t>
   </si>
   <si>
-    <t>{"weapons":[], "armor":[]}</t>
+    <t>{"weapons":[], "armor":[], "potions":[], "food":[], "misc":[]}</t>
+  </si>
+  <si>
+    <t>[]</t>
+  </si>
+  <si>
+    <t>Nature</t>
   </si>
 </sst>
 </file>
@@ -583,18 +589,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC346DE0-872D-4641-8919-23CF44305F87}">
-  <dimension ref="A1:G101"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="34.33203125" customWidth="1"/>
+    <col min="5" max="5" width="54.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -617,805 +623,18 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" cm="1">
-        <f t="array" ref="A2:A101">_xlfn.SEQUENCE(100)</f>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2">
         <v>1</v>
       </c>
       <c r="E2" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="E3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="E4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="E5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="E6" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="E7" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="E8" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="E9" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="E10" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="E11" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="E12" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="E13" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="E14" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="E15" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16">
-        <v>15</v>
-      </c>
-      <c r="E16" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17">
-        <v>16</v>
-      </c>
-      <c r="E17" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18">
-        <v>17</v>
-      </c>
-      <c r="E18" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19">
-        <v>18</v>
-      </c>
-      <c r="E19" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20">
-        <v>19</v>
-      </c>
-      <c r="E20" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21">
-        <v>20</v>
-      </c>
-      <c r="E21" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22">
-        <v>21</v>
-      </c>
-      <c r="E22" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23">
-        <v>22</v>
-      </c>
-      <c r="E23" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24">
-        <v>23</v>
-      </c>
-      <c r="E24" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25">
-        <v>24</v>
-      </c>
-      <c r="E25" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26">
-        <v>25</v>
-      </c>
-      <c r="E26" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27">
-        <v>26</v>
-      </c>
-      <c r="E27" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28">
-        <v>27</v>
-      </c>
-      <c r="E28" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29">
-        <v>28</v>
-      </c>
-      <c r="E29" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A30">
-        <v>29</v>
-      </c>
-      <c r="E30" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A31">
-        <v>30</v>
-      </c>
-      <c r="E31" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A32">
-        <v>31</v>
-      </c>
-      <c r="E32" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A33">
-        <v>32</v>
-      </c>
-      <c r="E33" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A34">
-        <v>33</v>
-      </c>
-      <c r="E34" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A35">
-        <v>34</v>
-      </c>
-      <c r="E35" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A36">
-        <v>35</v>
-      </c>
-      <c r="E36" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A37">
-        <v>36</v>
-      </c>
-      <c r="E37" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A38">
-        <v>37</v>
-      </c>
-      <c r="E38" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A39">
-        <v>38</v>
-      </c>
-      <c r="E39" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A40">
-        <v>39</v>
-      </c>
-      <c r="E40" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A41">
-        <v>40</v>
-      </c>
-      <c r="E41" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A42">
-        <v>41</v>
-      </c>
-      <c r="E42" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A43">
-        <v>42</v>
-      </c>
-      <c r="E43" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A44">
-        <v>43</v>
-      </c>
-      <c r="E44" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A45">
-        <v>44</v>
-      </c>
-      <c r="E45" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A46">
-        <v>45</v>
-      </c>
-      <c r="E46" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A47">
-        <v>46</v>
-      </c>
-      <c r="E47" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A48">
-        <v>47</v>
-      </c>
-      <c r="E48" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A49">
-        <v>48</v>
-      </c>
-      <c r="E49" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A50">
+      <c r="F2" t="s">
         <v>49</v>
       </c>
-      <c r="E50" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A51">
-        <v>50</v>
-      </c>
-      <c r="E51" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A52">
-        <v>51</v>
-      </c>
-      <c r="E52" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A53">
-        <v>52</v>
-      </c>
-      <c r="E53" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A54">
-        <v>53</v>
-      </c>
-      <c r="E54" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A55">
-        <v>54</v>
-      </c>
-      <c r="E55" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A56">
-        <v>55</v>
-      </c>
-      <c r="E56" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A57">
-        <v>56</v>
-      </c>
-      <c r="E57" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A58">
-        <v>57</v>
-      </c>
-      <c r="E58" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A59">
-        <v>58</v>
-      </c>
-      <c r="E59" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A60">
-        <v>59</v>
-      </c>
-      <c r="E60" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A61">
-        <v>60</v>
-      </c>
-      <c r="E61" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A62">
-        <v>61</v>
-      </c>
-      <c r="E62" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A63">
-        <v>62</v>
-      </c>
-      <c r="E63" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A64">
-        <v>63</v>
-      </c>
-      <c r="E64" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A65">
-        <v>64</v>
-      </c>
-      <c r="E65" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A66">
-        <v>65</v>
-      </c>
-      <c r="E66" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A67">
-        <v>66</v>
-      </c>
-      <c r="E67" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A68">
-        <v>67</v>
-      </c>
-      <c r="E68" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A69">
-        <v>68</v>
-      </c>
-      <c r="E69" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A70">
-        <v>69</v>
-      </c>
-      <c r="E70" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A71">
-        <v>70</v>
-      </c>
-      <c r="E71" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A72">
-        <v>71</v>
-      </c>
-      <c r="E72" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A73">
-        <v>72</v>
-      </c>
-      <c r="E73" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A74">
-        <v>73</v>
-      </c>
-      <c r="E74" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A75">
-        <v>74</v>
-      </c>
-      <c r="E75" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A76">
-        <v>75</v>
-      </c>
-      <c r="E76" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A77">
-        <v>76</v>
-      </c>
-      <c r="E77" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A78">
-        <v>77</v>
-      </c>
-      <c r="E78" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A79">
-        <v>78</v>
-      </c>
-      <c r="E79" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A80">
-        <v>79</v>
-      </c>
-      <c r="E80" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A81">
-        <v>80</v>
-      </c>
-      <c r="E81" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A82">
-        <v>81</v>
-      </c>
-      <c r="E82" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A83">
-        <v>82</v>
-      </c>
-      <c r="E83" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A84">
-        <v>83</v>
-      </c>
-      <c r="E84" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A85">
-        <v>84</v>
-      </c>
-      <c r="E85" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A86">
-        <v>85</v>
-      </c>
-      <c r="E86" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A87">
-        <v>86</v>
-      </c>
-      <c r="E87" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A88">
-        <v>87</v>
-      </c>
-      <c r="E88" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A89">
-        <v>88</v>
-      </c>
-      <c r="E89" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A90">
-        <v>89</v>
-      </c>
-      <c r="E90" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A91">
-        <v>90</v>
-      </c>
-      <c r="E91" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A92">
-        <v>91</v>
-      </c>
-      <c r="E92" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A93">
-        <v>92</v>
-      </c>
-      <c r="E93" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A94">
-        <v>93</v>
-      </c>
-      <c r="E94" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A95">
-        <v>94</v>
-      </c>
-      <c r="E95" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A96">
-        <v>95</v>
-      </c>
-      <c r="E96" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A97">
-        <v>96</v>
-      </c>
-      <c r="E97" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A98">
-        <v>97</v>
-      </c>
-      <c r="E98" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A99">
-        <v>98</v>
-      </c>
-      <c r="E99" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A100">
-        <v>99</v>
-      </c>
-      <c r="E100" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A101">
-        <v>100</v>
-      </c>
-      <c r="E101" t="s">
-        <v>48</v>
+      <c r="G2" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -1429,7 +648,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1443,18 +662,18 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" style="5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1489,7 +708,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="3" cm="1">
         <f t="array" ref="A2:A101">_xlfn.SEQUENCE(100)</f>
         <v>1</v>
@@ -1525,7 +744,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -1560,7 +779,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -1595,487 +814,487 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" s="3">
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" s="3">
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" s="3">
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" s="3">
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="3">
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" s="3">
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="3">
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" s="3">
         <v>51</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" s="3">
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" s="3">
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" s="3">
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" s="3">
         <v>55</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" s="3">
         <v>56</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" s="3">
         <v>57</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" s="3">
         <v>58</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" s="3">
         <v>59</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" s="3">
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" s="3">
         <v>61</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" s="3">
         <v>62</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" s="3">
         <v>63</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" s="3">
         <v>64</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" s="3">
         <v>65</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" s="3">
         <v>66</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" s="3">
         <v>67</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" s="3">
         <v>68</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" s="3">
         <v>69</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" s="3">
         <v>70</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" s="3">
         <v>71</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" s="3">
         <v>72</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" s="3">
         <v>73</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" s="3">
         <v>74</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" s="3">
         <v>75</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77" s="3">
         <v>76</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78" s="3">
         <v>77</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79" s="3">
         <v>78</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80" s="3">
         <v>79</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81" s="3">
         <v>80</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" s="3">
         <v>81</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83" s="3">
         <v>82</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84" s="3">
         <v>83</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85" s="3">
         <v>84</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86" s="3">
         <v>85</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87" s="3">
         <v>86</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88" s="3">
         <v>87</v>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89" s="3">
         <v>88</v>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A90" s="3">
         <v>89</v>
       </c>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91" s="3">
         <v>90</v>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92" s="3">
         <v>91</v>
       </c>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93" s="3">
         <v>92</v>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A94" s="3">
         <v>93</v>
       </c>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A95" s="3">
         <v>94</v>
       </c>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A96" s="3">
         <v>95</v>
       </c>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97" s="3">
         <v>96</v>
       </c>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98" s="3">
         <v>97</v>
       </c>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99" s="3">
         <v>98</v>
       </c>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100" s="3">
         <v>99</v>
       </c>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A101" s="3">
         <v>100</v>
       </c>
@@ -2091,16 +1310,16 @@
   <dimension ref="A1:E101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2117,7 +1336,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="3" cm="1">
         <f t="array" ref="A2:A101">_xlfn.SEQUENCE(100)</f>
         <v>1</v>
@@ -2128,498 +1347,504 @@
       <c r="C2">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" s="3">
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" s="3">
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" s="3">
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" s="3">
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="3">
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" s="3">
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="3">
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" s="3">
         <v>51</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" s="3">
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" s="3">
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" s="3">
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" s="3">
         <v>55</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" s="3">
         <v>56</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" s="3">
         <v>57</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" s="3">
         <v>58</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" s="3">
         <v>59</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" s="3">
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" s="3">
         <v>61</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" s="3">
         <v>62</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" s="3">
         <v>63</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" s="3">
         <v>64</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" s="3">
         <v>65</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" s="3">
         <v>66</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" s="3">
         <v>67</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" s="3">
         <v>68</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" s="3">
         <v>69</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" s="3">
         <v>70</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" s="3">
         <v>71</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" s="3">
         <v>72</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" s="3">
         <v>73</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" s="3">
         <v>74</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" s="3">
         <v>75</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77" s="3">
         <v>76</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78" s="3">
         <v>77</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79" s="3">
         <v>78</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80" s="3">
         <v>79</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81" s="3">
         <v>80</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" s="3">
         <v>81</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83" s="3">
         <v>82</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84" s="3">
         <v>83</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85" s="3">
         <v>84</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86" s="3">
         <v>85</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87" s="3">
         <v>86</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88" s="3">
         <v>87</v>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89" s="3">
         <v>88</v>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A90" s="3">
         <v>89</v>
       </c>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91" s="3">
         <v>90</v>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92" s="3">
         <v>91</v>
       </c>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93" s="3">
         <v>92</v>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A94" s="3">
         <v>93</v>
       </c>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A95" s="3">
         <v>94</v>
       </c>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A96" s="3">
         <v>95</v>
       </c>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97" s="3">
         <v>96</v>
       </c>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98" s="3">
         <v>97</v>
       </c>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99" s="3">
         <v>98</v>
       </c>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100" s="3">
         <v>99</v>
       </c>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A101" s="3">
         <v>100</v>
       </c>
@@ -2635,23 +1860,23 @@
   <dimension ref="A1:J101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="4.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2683,7 +1908,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" cm="1">
         <f t="array" ref="A2:A101">_xlfn.SEQUENCE(100)</f>
         <v>1</v>
@@ -2692,7 +1917,7 @@
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>49</v>
       </c>
       <c r="E2">
         <v>-1</v>
@@ -2713,7 +1938,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2721,7 +1946,7 @@
         <v>15</v>
       </c>
       <c r="D3" t="s">
-        <v>10</v>
+        <v>49</v>
       </c>
       <c r="E3">
         <v>-1</v>
@@ -2742,7 +1967,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2750,7 +1975,7 @@
         <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>10</v>
+        <v>49</v>
       </c>
       <c r="E4">
         <v>-1</v>
@@ -2771,7 +1996,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2779,7 +2004,7 @@
         <v>17</v>
       </c>
       <c r="D5" t="s">
-        <v>10</v>
+        <v>49</v>
       </c>
       <c r="E5">
         <v>-1</v>
@@ -2800,7 +2025,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2808,7 +2033,7 @@
         <v>18</v>
       </c>
       <c r="D6" t="s">
-        <v>10</v>
+        <v>49</v>
       </c>
       <c r="E6">
         <v>-1</v>
@@ -2829,477 +2054,477 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>55</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>56</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>57</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>58</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>59</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>61</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>62</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>63</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>64</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>65</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>66</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>67</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>68</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>69</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>70</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>71</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>72</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>73</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>74</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>75</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>76</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>77</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>78</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>79</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>80</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>81</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>82</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>83</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>84</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>85</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>86</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>87</v>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>88</v>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>89</v>
       </c>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>90</v>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>91</v>
       </c>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>92</v>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>93</v>
       </c>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>94</v>
       </c>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>95</v>
       </c>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>96</v>
       </c>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>97</v>
       </c>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>98</v>
       </c>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>99</v>
       </c>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>100</v>
       </c>
@@ -3318,12 +2543,12 @@
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3343,7 +2568,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" cm="1">
         <f t="array" ref="A2:A101">_xlfn.SEQUENCE(100)</f>
         <v>1</v>
@@ -3364,7 +2589,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3384,7 +2609,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -3404,7 +2629,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -3424,482 +2649,482 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>55</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>56</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>57</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>58</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>59</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>61</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>62</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>63</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>64</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>65</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>66</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>67</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>68</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>69</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>70</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>71</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>72</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>73</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>74</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>75</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>76</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>77</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>78</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>79</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>80</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>81</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>82</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>83</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>84</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>85</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>86</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>87</v>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>88</v>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>89</v>
       </c>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>90</v>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>91</v>
       </c>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>92</v>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>93</v>
       </c>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>94</v>
       </c>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>95</v>
       </c>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>96</v>
       </c>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>97</v>
       </c>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>98</v>
       </c>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>99</v>
       </c>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>100</v>
       </c>
@@ -3917,9 +3142,9 @@
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -3933,7 +3158,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3" cm="1">
         <f t="array" ref="A2:A101">_xlfn.SEQUENCE(100)</f>
         <v>1</v>
@@ -3948,497 +3173,497 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>55</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>56</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>57</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>58</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>59</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>61</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>62</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>63</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>64</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>65</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>66</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>67</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>68</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>69</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>70</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>71</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>72</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>73</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>74</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>75</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>76</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>77</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>78</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>79</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>80</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>81</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>82</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>83</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>84</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>85</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>86</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>87</v>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>88</v>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>89</v>
       </c>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>90</v>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>91</v>
       </c>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>92</v>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>93</v>
       </c>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>94</v>
       </c>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>95</v>
       </c>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>96</v>
       </c>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>97</v>
       </c>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>98</v>
       </c>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>99</v>
       </c>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>100</v>
       </c>
@@ -4456,9 +3681,9 @@
       <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4492,9 +3717,9 @@
       <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4523,7 +3748,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -4564,9 +3789,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>

</xml_diff>